<commit_message>
Attempting to fit dilution function for Bz
</commit_message>
<xml_diff>
--- a/RadialFieldOps_2/RadialFieldScan_2.xlsx
+++ b/RadialFieldOps_2/RadialFieldScan_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/RadialFieldOps_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ABFBF2-3124-3649-AD09-AF6FD86488E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF590FF6-8FC3-F04C-9F69-F83D3B5BFE11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{3DAFEA06-3AA8-BB44-8E27-DDA65B3686C5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{3DAFEA06-3AA8-BB44-8E27-DDA65B3686C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4313,8 +4313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B752E6E-F960-2F47-AC55-2B0104D935A3}">
   <dimension ref="A2:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6652,7 +6652,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>